<commit_message>
Updated Schedule for Iter1
</commit_message>
<xml_diff>
--- a/IS212_Schedule_G5T4.xlsx
+++ b/IS212_Schedule_G5T4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD72612F-E2D8-45DE-92FF-76B2BD3C5139}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E73B65-E874-4022-B98A-104565FD0A12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -508,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -629,6 +629,12 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -918,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="98" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,25 +992,25 @@
       <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="44">
         <v>43722.416666666664</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="44">
         <v>43722.489583333336</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="43">
         <v>1.75</v>
       </c>
-      <c r="G2" s="42">
+      <c r="G2" s="44">
         <v>43722.416666666664</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="44">
         <v>43722.489583333336</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2" s="43">
         <v>1.75</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="43" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="20" t="s">
@@ -1024,13 +1030,13 @@
       <c r="C3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="20" t="s">
         <v>9</v>
       </c>
@@ -1048,13 +1054,13 @@
       <c r="C4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
       <c r="K4" s="20" t="s">
         <v>9</v>
       </c>
@@ -1072,13 +1078,13 @@
       <c r="C5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
       <c r="K5" s="20" t="s">
         <v>9</v>
       </c>
@@ -1096,13 +1102,13 @@
       <c r="C6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="20" t="s">
         <v>9</v>
       </c>
@@ -1129,15 +1135,21 @@
       <c r="F7" s="20">
         <v>1</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="42">
+        <v>43724.708333333336</v>
+      </c>
+      <c r="H7" s="42">
+        <v>43724.75</v>
+      </c>
       <c r="I7" s="24">
         <v>1</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="25"/>
+      <c r="K7" s="41" t="s">
+        <v>9</v>
+      </c>
       <c r="L7" s="20" t="s">
         <v>17</v>
       </c>
@@ -1161,13 +1173,21 @@
       <c r="F8" s="20">
         <v>1</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
+      <c r="G8" s="42">
+        <v>43724.75</v>
+      </c>
+      <c r="H8" s="42">
+        <v>43724.791666666664</v>
+      </c>
+      <c r="I8" s="41">
+        <v>1</v>
+      </c>
       <c r="J8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="25"/>
+      <c r="K8" s="41" t="s">
+        <v>9</v>
+      </c>
       <c r="L8" s="20" t="s">
         <v>17</v>
       </c>
@@ -1191,13 +1211,21 @@
       <c r="F9" s="20">
         <v>0.25</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="25"/>
+      <c r="G9" s="42">
+        <v>43724.791666666664</v>
+      </c>
+      <c r="H9" s="42">
+        <v>43724.802083333336</v>
+      </c>
+      <c r="I9" s="41">
+        <v>0.25</v>
+      </c>
       <c r="J9" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="25"/>
+      <c r="K9" s="41" t="s">
+        <v>9</v>
+      </c>
       <c r="L9" s="20" t="s">
         <v>17</v>
       </c>
@@ -1221,13 +1249,21 @@
       <c r="F10" s="20">
         <v>2</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="25"/>
+      <c r="G10" s="28">
+        <v>43725.75</v>
+      </c>
+      <c r="H10" s="28">
+        <v>43725.833333333336</v>
+      </c>
+      <c r="I10" s="41">
+        <v>2</v>
+      </c>
       <c r="J10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="41" t="s">
+        <v>9</v>
+      </c>
       <c r="L10" s="29" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Update Schedule for Pair Programming
</commit_message>
<xml_diff>
--- a/IS212_Schedule_G5T4.xlsx
+++ b/IS212_Schedule_G5T4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E73B65-E874-4022-B98A-104565FD0A12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12BA9C4-B8A7-437F-BB17-D9B5AC554B68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -508,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -635,6 +635,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -924,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -992,25 +995,25 @@
       <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="45">
         <v>43722.416666666664</v>
       </c>
-      <c r="E2" s="44">
+      <c r="E2" s="45">
         <v>43722.489583333336</v>
       </c>
-      <c r="F2" s="43">
+      <c r="F2" s="44">
         <v>1.75</v>
       </c>
-      <c r="G2" s="44">
+      <c r="G2" s="45">
         <v>43722.416666666664</v>
       </c>
-      <c r="H2" s="44">
+      <c r="H2" s="45">
         <v>43722.489583333336</v>
       </c>
-      <c r="I2" s="43">
+      <c r="I2" s="44">
         <v>1.75</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="44" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="20" t="s">
@@ -1030,13 +1033,13 @@
       <c r="C3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="20" t="s">
         <v>9</v>
       </c>
@@ -1054,13 +1057,13 @@
       <c r="C4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
       <c r="K4" s="20" t="s">
         <v>9</v>
       </c>
@@ -1078,13 +1081,13 @@
       <c r="C5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
       <c r="K5" s="20" t="s">
         <v>9</v>
       </c>
@@ -1102,13 +1105,13 @@
       <c r="C6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
       <c r="K6" s="20" t="s">
         <v>9</v>
       </c>
@@ -1287,13 +1290,21 @@
       <c r="F11" s="20">
         <v>2</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="25"/>
+      <c r="G11" s="28">
+        <v>43726.5</v>
+      </c>
+      <c r="H11" s="28">
+        <v>43726.583333333336</v>
+      </c>
+      <c r="I11" s="43">
+        <v>2</v>
+      </c>
       <c r="J11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="43" t="s">
+        <v>9</v>
+      </c>
       <c r="L11" s="29" t="s">
         <v>21</v>
       </c>

</xml_diff>